<commit_message>
feat: créer une fonction pour paramétrer l'affichage de la caption sous le graphique
</commit_message>
<xml_diff>
--- a/inegalites/data/tab_inegalites.xlsx
+++ b/inegalites/data/tab_inegalites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mouna/Desktop/Work/GitHub/cereq-dataviz/inegalites/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1828672-4CA5-1946-9C81-1CFE135778C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A438D8C6-2CD6-2940-87B6-8D6BB2C3FE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20140" xr2:uid="{6ABDD48A-BC5F-46EA-ABB7-F3EFE135F388}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26020" xr2:uid="{6ABDD48A-BC5F-46EA-ABB7-F3EFE135F388}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -155,12 +155,6 @@
     <t>Ménages à dominante ouvrière</t>
   </si>
   <si>
-    <t>Ménages d'un employé ou ouvrier</t>
-  </si>
-  <si>
-    <t>Ménages d'inactifs</t>
-  </si>
-  <si>
     <t>ascendance migratoire</t>
   </si>
   <si>
@@ -173,18 +167,6 @@
     <t>Autres immigrés</t>
   </si>
   <si>
-    <t>Nés en France ayant au moins un parent immigré d'Europe</t>
-  </si>
-  <si>
-    <t>Nés en France ayant au moins un parent immigré d'Afrique</t>
-  </si>
-  <si>
-    <t>Nés en France ayant au moins un parent immigré d'autres régions que l'Afrique et l'Europe</t>
-  </si>
-  <si>
-    <t>Autres cas (Parents français nés à l'étranger, origine des parents inconnues, etc.)</t>
-  </si>
-  <si>
     <t>lieu de résidence à la fin des études</t>
   </si>
   <si>
@@ -192,6 +174,24 @@
   </si>
   <si>
     <t>Hors dun quartier prioritaire de la ville</t>
+  </si>
+  <si>
+    <t>Ménages dun employé ou ouvrier</t>
+  </si>
+  <si>
+    <t>Ménages dinactifs</t>
+  </si>
+  <si>
+    <t>Nés en France ayant au moins un parent immigré dEurope</t>
+  </si>
+  <si>
+    <t>Nés en France ayant au moins un parent immigré dAfrique</t>
+  </si>
+  <si>
+    <t>Nés en France ayant au moins un parent immigré dautres régions que lAfrique et lEurope</t>
+  </si>
+  <si>
+    <t>Autres cas (Parents français nés à létranger, origine des parents inconnues, etc.)</t>
   </si>
 </sst>
 </file>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1D79A9-222A-4134-802A-F0F64B64E71D}">
   <dimension ref="A1:U187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2916,7 +2916,7 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C37">
         <v>6</v>
@@ -2981,7 +2981,7 @@
         <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C38">
         <v>13</v>
@@ -3046,7 +3046,7 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C39">
         <v>20</v>
@@ -3111,7 +3111,7 @@
         <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C40">
         <v>27</v>
@@ -3176,7 +3176,7 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C41">
         <v>34</v>
@@ -3241,7 +3241,7 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>7</v>
@@ -3306,7 +3306,7 @@
         <v>33</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C43">
         <v>14</v>
@@ -3371,7 +3371,7 @@
         <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C44">
         <v>21</v>
@@ -3436,7 +3436,7 @@
         <v>33</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C45">
         <v>28</v>
@@ -3501,7 +3501,7 @@
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C46">
         <v>35</v>
@@ -3563,10 +3563,10 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -3628,10 +3628,10 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C48">
         <v>8</v>
@@ -3693,10 +3693,10 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C49">
         <v>15</v>
@@ -3758,10 +3758,10 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C50">
         <v>22</v>
@@ -3823,10 +3823,10 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C51">
         <v>29</v>
@@ -3888,10 +3888,10 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" t="s">
         <v>41</v>
-      </c>
-      <c r="B52" t="s">
-        <v>43</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -3953,10 +3953,10 @@
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" t="s">
         <v>41</v>
-      </c>
-      <c r="B53" t="s">
-        <v>43</v>
       </c>
       <c r="C53">
         <v>9</v>
@@ -4018,10 +4018,10 @@
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B54" t="s">
         <v>41</v>
-      </c>
-      <c r="B54" t="s">
-        <v>43</v>
       </c>
       <c r="C54">
         <v>16</v>
@@ -4083,10 +4083,10 @@
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>39</v>
+      </c>
+      <c r="B55" t="s">
         <v>41</v>
-      </c>
-      <c r="B55" t="s">
-        <v>43</v>
       </c>
       <c r="C55">
         <v>23</v>
@@ -4148,10 +4148,10 @@
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" t="s">
         <v>41</v>
-      </c>
-      <c r="B56" t="s">
-        <v>43</v>
       </c>
       <c r="C56">
         <v>30</v>
@@ -4213,10 +4213,10 @@
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C57">
         <v>3</v>
@@ -4278,10 +4278,10 @@
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C58">
         <v>10</v>
@@ -4343,10 +4343,10 @@
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C59">
         <v>17</v>
@@ -4408,10 +4408,10 @@
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B60" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C60">
         <v>24</v>
@@ -4473,10 +4473,10 @@
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C61">
         <v>31</v>
@@ -4538,10 +4538,10 @@
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B62" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C62">
         <v>4</v>
@@ -4603,10 +4603,10 @@
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B63" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C63">
         <v>11</v>
@@ -4668,10 +4668,10 @@
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B64" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C64">
         <v>18</v>
@@ -4733,10 +4733,10 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B65" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C65">
         <v>25</v>
@@ -4798,10 +4798,10 @@
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B66" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C66">
         <v>32</v>
@@ -4863,10 +4863,10 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B67" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C67">
         <v>5</v>
@@ -4928,10 +4928,10 @@
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B68" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C68">
         <v>12</v>
@@ -4993,10 +4993,10 @@
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C69">
         <v>19</v>
@@ -5058,10 +5058,10 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B70" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C70">
         <v>26</v>
@@ -5123,10 +5123,10 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B71" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C71">
         <v>33</v>
@@ -5188,10 +5188,10 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B72" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C72">
         <v>6</v>
@@ -5253,10 +5253,10 @@
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B73" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C73">
         <v>13</v>
@@ -5318,10 +5318,10 @@
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B74" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C74">
         <v>20</v>
@@ -5383,10 +5383,10 @@
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B75" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C75">
         <v>27</v>
@@ -5448,10 +5448,10 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B76" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C76">
         <v>34</v>
@@ -5513,10 +5513,10 @@
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B77" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C77">
         <v>7</v>
@@ -5578,10 +5578,10 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B78" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C78">
         <v>14</v>
@@ -5643,10 +5643,10 @@
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C79">
         <v>21</v>
@@ -5708,10 +5708,10 @@
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C80">
         <v>28</v>
@@ -5773,10 +5773,10 @@
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B81" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C81">
         <v>35</v>
@@ -5838,10 +5838,10 @@
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B82" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -5903,10 +5903,10 @@
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B83" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -5968,10 +5968,10 @@
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B84" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C84">
         <v>5</v>
@@ -6033,10 +6033,10 @@
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B85" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C85">
         <v>7</v>
@@ -6098,10 +6098,10 @@
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B86" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C86">
         <v>9</v>
@@ -6163,10 +6163,10 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B87" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C87">
         <v>2</v>
@@ -6228,10 +6228,10 @@
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B88" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C88">
         <v>4</v>
@@ -6293,10 +6293,10 @@
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B89" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C89">
         <v>6</v>
@@ -6358,10 +6358,10 @@
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B90" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C90">
         <v>8</v>
@@ -6423,10 +6423,10 @@
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B91" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C91">
         <v>10</v>
@@ -6488,7 +6488,7 @@
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -6497,6 +6497,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000DCE2AD71575ED409F6CD8D87660A7B5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="426d87b04946fef7e3a4dc34d3d122df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a3559f96-a391-4298-a476-5fa029e2109e" xmlns:ns3="e8254419-5e3e-4d09-9ab1-694bd035361a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="241cc2e6b550b1a0bc2d3e1e684e1cae" ns2:_="" ns3:_="">
     <xsd:import namespace="a3559f96-a391-4298-a476-5fa029e2109e"/>
@@ -6719,15 +6728,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6740,6 +6740,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5447FCD1-6D4E-4F26-8984-075EA9AA1E5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C200FC9-CFF6-4177-B141-1E80222EFE5C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6754,14 +6762,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5447FCD1-6D4E-4F26-8984-075EA9AA1E5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: créer une fonction pour paramétrer les couleurs des barres en fonction du nombre de modalités
</commit_message>
<xml_diff>
--- a/inegalites/data/tab_inegalites.xlsx
+++ b/inegalites/data/tab_inegalites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mouna/Desktop/Work/GitHub/cereq-dataviz/inegalites/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A438D8C6-2CD6-2940-87B6-8D6BB2C3FE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B04D294-15A7-6242-89ED-B2F42000FC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26020" xr2:uid="{6ABDD48A-BC5F-46EA-ABB7-F3EFE135F388}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="25960" xr2:uid="{6ABDD48A-BC5F-46EA-ABB7-F3EFE135F388}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="52">
   <si>
     <t>facteur_analyse</t>
   </si>
@@ -550,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1D79A9-222A-4134-802A-F0F64B64E71D}">
-  <dimension ref="A1:U187"/>
+  <dimension ref="A1:U91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6486,26 +6486,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000DCE2AD71575ED409F6CD8D87660A7B5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="426d87b04946fef7e3a4dc34d3d122df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a3559f96-a391-4298-a476-5fa029e2109e" xmlns:ns3="e8254419-5e3e-4d09-9ab1-694bd035361a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="241cc2e6b550b1a0bc2d3e1e684e1cae" ns2:_="" ns3:_="">
     <xsd:import namespace="a3559f96-a391-4298-a476-5fa029e2109e"/>
@@ -6728,6 +6714,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6740,14 +6735,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5447FCD1-6D4E-4F26-8984-075EA9AA1E5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C200FC9-CFF6-4177-B141-1E80222EFE5C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6762,6 +6749,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5447FCD1-6D4E-4F26-8984-075EA9AA1E5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>